<commit_message>
UUID for subgroup in the Convictions Data Structure changed.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy(Data-Structures)_V1.0.3.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy(Data-Structures)_V1.0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="351">
   <si>
     <t>005eb9ed-1347-4ca3-bb29-9bc0db64e1ab</t>
   </si>
@@ -1099,13 +1099,16 @@
   </si>
   <si>
     <t>f5276600-a2b6-4ff6-a90e-b31fe19dae41</t>
+  </si>
+  <si>
+    <t>f4978772-3126-4ded-bc30-f50da8c3a038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1269,6 +1272,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1696,7 +1705,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1752,6 +1761,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2456,8 +2468,8 @@
       <c r="M10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="21" t="s">
-        <v>26</v>
+      <c r="N10" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
@@ -2947,8 +2959,8 @@
       <c r="M28" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="N28" s="21" t="s">
-        <v>26</v>
+      <c r="N28" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
@@ -3438,8 +3450,8 @@
       <c r="M46" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N46" s="21" t="s">
-        <v>26</v>
+      <c r="N46" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
@@ -3929,8 +3941,8 @@
       <c r="M64" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N64" s="21" t="s">
-        <v>26</v>
+      <c r="N64" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O64" s="27"/>
       <c r="P64" s="27"/>
@@ -4420,8 +4432,8 @@
       <c r="M82" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="N82" s="21" t="s">
-        <v>26</v>
+      <c r="N82" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O82" s="27"/>
       <c r="P82" s="27"/>
@@ -4911,8 +4923,8 @@
       <c r="M100" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N100" s="21" t="s">
-        <v>26</v>
+      <c r="N100" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="O100" s="27"/>
       <c r="P100" s="27"/>

</xml_diff>